<commit_message>
updating the FIM code
</commit_message>
<xml_diff>
--- a/inst/extdata/projections.xlsx
+++ b/inst/extdata/projections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahmad\Downloads\FIM\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GNabors\Downloads\fim\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948DE6D3-751E-450A-B349-7FEAD4A506AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD50D6C-D498-46D0-9E3F-0F5388F6C4EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionary" sheetId="12" r:id="rId1"/>
@@ -9676,14 +9676,14 @@
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.58203125" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" style="36" customWidth="1"/>
-    <col min="4" max="5" width="19.58203125" customWidth="1"/>
+    <col min="1" max="2" width="19.625" customWidth="1"/>
+    <col min="3" max="3" width="26.375" style="36" customWidth="1"/>
+    <col min="4" max="5" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47" t="s">
         <v>277</v>
       </c>
@@ -9711,7 +9711,7 @@
       <c r="O1" s="39"/>
       <c r="P1" s="39"/>
     </row>
-    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
         <v>278</v>
       </c>
@@ -9739,7 +9739,7 @@
       <c r="O2" s="41"/>
       <c r="P2" s="42"/>
     </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66"/>
       <c r="B3" s="63"/>
       <c r="C3" s="63"/>
@@ -9761,7 +9761,7 @@
       <c r="O3" s="43"/>
       <c r="P3" s="44"/>
     </row>
-    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="66"/>
       <c r="B4" s="63"/>
       <c r="C4" s="63"/>
@@ -9783,7 +9783,7 @@
       <c r="O4" s="43"/>
       <c r="P4" s="44"/>
     </row>
-    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="66"/>
       <c r="B5" s="63"/>
       <c r="C5" s="63"/>
@@ -9805,7 +9805,7 @@
       <c r="O5" s="43"/>
       <c r="P5" s="44"/>
     </row>
-    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="66"/>
       <c r="B6" s="63"/>
       <c r="C6" s="63"/>
@@ -9827,7 +9827,7 @@
       <c r="O6" s="43"/>
       <c r="P6" s="44"/>
     </row>
-    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="66"/>
       <c r="B7" s="63"/>
       <c r="C7" s="63"/>
@@ -9849,7 +9849,7 @@
       <c r="O7" s="43"/>
       <c r="P7" s="44"/>
     </row>
-    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="66"/>
       <c r="B8" s="63"/>
       <c r="C8" s="63"/>
@@ -9871,7 +9871,7 @@
       <c r="O8" s="43"/>
       <c r="P8" s="44"/>
     </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="66"/>
       <c r="B9" s="63"/>
       <c r="C9" s="63"/>
@@ -9893,7 +9893,7 @@
       <c r="O9" s="43"/>
       <c r="P9" s="44"/>
     </row>
-    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="66"/>
       <c r="B10" s="63"/>
       <c r="C10" s="63"/>
@@ -9915,7 +9915,7 @@
       <c r="O10" s="43"/>
       <c r="P10" s="44"/>
     </row>
-    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="66"/>
       <c r="B11" s="63"/>
       <c r="C11" s="63"/>
@@ -9937,7 +9937,7 @@
       <c r="O11" s="43"/>
       <c r="P11" s="44"/>
     </row>
-    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="66"/>
       <c r="B12" s="63"/>
       <c r="C12" s="63"/>
@@ -9959,7 +9959,7 @@
       <c r="O12" s="43"/>
       <c r="P12" s="44"/>
     </row>
-    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="66"/>
       <c r="B13" s="63"/>
       <c r="C13" s="63"/>
@@ -9981,7 +9981,7 @@
       <c r="O13" s="43"/>
       <c r="P13" s="44"/>
     </row>
-    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="66"/>
       <c r="B14" s="63"/>
       <c r="C14" s="63"/>
@@ -10003,7 +10003,7 @@
       <c r="O14" s="43"/>
       <c r="P14" s="44"/>
     </row>
-    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="66"/>
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
@@ -10025,7 +10025,7 @@
       <c r="O15" s="43"/>
       <c r="P15" s="44"/>
     </row>
-    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="66"/>
       <c r="B16" s="63"/>
       <c r="C16" s="63"/>
@@ -10047,7 +10047,7 @@
       <c r="O16" s="43"/>
       <c r="P16" s="44"/>
     </row>
-    <row r="17" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="67"/>
       <c r="B17" s="64"/>
       <c r="C17" s="64"/>
@@ -10069,7 +10069,7 @@
       <c r="O17" s="45"/>
       <c r="P17" s="46"/>
     </row>
-    <row r="18" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="65" t="s">
         <v>282</v>
       </c>
@@ -10097,7 +10097,7 @@
       <c r="O18" s="41"/>
       <c r="P18" s="42"/>
     </row>
-    <row r="19" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="66"/>
       <c r="B19" s="63"/>
       <c r="C19" s="63"/>
@@ -10119,7 +10119,7 @@
       <c r="O19" s="43"/>
       <c r="P19" s="44"/>
     </row>
-    <row r="20" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="66"/>
       <c r="B20" s="63"/>
       <c r="C20" s="63"/>
@@ -10141,7 +10141,7 @@
       <c r="O20" s="43"/>
       <c r="P20" s="44"/>
     </row>
-    <row r="21" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="66"/>
       <c r="B21" s="63"/>
       <c r="C21" s="64"/>
@@ -10163,7 +10163,7 @@
       <c r="O21" s="45"/>
       <c r="P21" s="46"/>
     </row>
-    <row r="22" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="66"/>
       <c r="B22" s="63"/>
       <c r="C22" s="63" t="s">
@@ -10187,7 +10187,7 @@
       <c r="O22" s="43"/>
       <c r="P22" s="44"/>
     </row>
-    <row r="23" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="66"/>
       <c r="B23" s="63"/>
       <c r="C23" s="63"/>
@@ -10209,7 +10209,7 @@
       <c r="O23" s="43"/>
       <c r="P23" s="44"/>
     </row>
-    <row r="24" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="66"/>
       <c r="B24" s="63"/>
       <c r="C24" s="63"/>
@@ -10231,7 +10231,7 @@
       <c r="O24" s="43"/>
       <c r="P24" s="44"/>
     </row>
-    <row r="25" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="67"/>
       <c r="B25" s="64"/>
       <c r="C25" s="64"/>
@@ -10253,7 +10253,7 @@
       <c r="O25" s="45"/>
       <c r="P25" s="46"/>
     </row>
-    <row r="27" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>308</v>
       </c>
@@ -10270,7 +10270,7 @@
       <c r="Q27" s="52"/>
       <c r="R27" s="52"/>
     </row>
-    <row r="28" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>309</v>
       </c>
@@ -10287,7 +10287,7 @@
       <c r="Q28" s="52"/>
       <c r="R28" s="52"/>
     </row>
-    <row r="29" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>310</v>
       </c>
@@ -10328,7 +10328,7 @@
         <v>2478.1</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>311</v>
       </c>
@@ -10369,7 +10369,7 @@
         <v>3235.2060000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>312</v>
       </c>
@@ -10410,7 +10410,7 @@
         <v>432.495</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G32" s="52">
         <v>615.77200000000005</v>
       </c>
@@ -10448,7 +10448,7 @@
         <v>932.56399999999996</v>
       </c>
     </row>
-    <row r="33" spans="7:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="7:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G33" s="31">
         <f>G29+G30+G31-G32</f>
         <v>2912.7670000000003</v>
@@ -10498,13 +10498,13 @@
         <v>5213.2370000000001</v>
       </c>
     </row>
-    <row r="40" spans="7:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="7:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I40" s="52"/>
       <c r="J40" s="52"/>
       <c r="K40" s="52"/>
       <c r="L40" s="52"/>
     </row>
-    <row r="41" spans="7:18" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="7:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I41" s="52"/>
       <c r="J41" s="52"/>
       <c r="K41" s="52"/>
@@ -10533,9 +10533,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2021</v>
       </c>
@@ -10612,12 +10612,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023</v>
       </c>
@@ -10638,7 +10638,7 @@
       <selection pane="bottomRight" activeCell="T38" sqref="T38:BL38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.75" style="2" customWidth="1"/>
     <col min="2" max="2" width="51.75" style="2" customWidth="1"/>
@@ -10649,12 +10649,12 @@
     <col min="61" max="16384" width="9.25" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="70" t="s">
         <v>156</v>
       </c>
@@ -10666,10 +10666,10 @@
       <c r="G2" s="71"/>
       <c r="H2" s="71"/>
     </row>
-    <row r="4" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="23"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="72" t="s">
         <v>155</v>
       </c>
@@ -10729,7 +10729,7 @@
       <c r="BG5" s="3"/>
       <c r="BH5" s="3"/>
     </row>
-    <row r="6" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="BA6" s="22"/>
       <c r="BB6" s="22"/>
       <c r="BC6" s="22"/>
@@ -10739,7 +10739,7 @@
       <c r="BK6" s="22"/>
       <c r="BL6" s="22"/>
     </row>
-    <row r="7" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -10927,7 +10927,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>93</v>
       </c>
@@ -11076,7 +11076,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>92</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>33695.9</v>
       </c>
     </row>
-    <row r="10" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>91</v>
       </c>
@@ -11452,7 +11452,7 @@
         <v>23545.3</v>
       </c>
     </row>
-    <row r="11" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="2" t="s">
         <v>90</v>
@@ -11641,7 +11641,7 @@
         <v>33795</v>
       </c>
     </row>
-    <row r="12" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="2" t="s">
         <v>89</v>
@@ -11830,7 +11830,7 @@
         <v>23615.3</v>
       </c>
     </row>
-    <row r="13" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>89</v>
       </c>
@@ -12018,7 +12018,7 @@
         <v>18628.5</v>
       </c>
     </row>
-    <row r="14" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
@@ -12203,7 +12203,7 @@
         <v>2.0049999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T15" s="16"/>
       <c r="U15" s="16"/>
       <c r="V15" s="16"/>
@@ -12250,7 +12250,7 @@
       <c r="BK15" s="16"/>
       <c r="BL15" s="16"/>
     </row>
-    <row r="16" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>88</v>
       </c>
@@ -12435,7 +12435,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="2" t="s">
         <v>86</v>
@@ -12624,7 +12624,7 @@
         <v>139.059</v>
       </c>
     </row>
-    <row r="18" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="D18" s="2" t="s">
         <v>20</v>
@@ -12810,7 +12810,7 @@
         <v>1.9910000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>85</v>
       </c>
@@ -12998,7 +12998,7 @@
         <v>141.75399999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="2" t="s">
         <v>20</v>
       </c>
@@ -13183,7 +13183,7 @@
         <v>2.0030000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>84</v>
       </c>
@@ -13371,7 +13371,7 @@
         <v>335.62799999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D22" s="2" t="s">
         <v>20</v>
       </c>
@@ -13556,7 +13556,7 @@
         <v>2.3069999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>83</v>
       </c>
@@ -13744,7 +13744,7 @@
         <v>346.53300000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D24" s="2" t="s">
         <v>20</v>
       </c>
@@ -13929,7 +13929,7 @@
         <v>2.3260000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>81</v>
       </c>
@@ -14117,7 +14117,7 @@
         <v>182.87299999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D26" s="2" t="s">
         <v>20</v>
       </c>
@@ -14302,7 +14302,7 @@
         <v>0.247</v>
       </c>
     </row>
-    <row r="27" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>79</v>
       </c>
@@ -14490,7 +14490,7 @@
         <v>143.11099999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D28" s="2" t="s">
         <v>20</v>
       </c>
@@ -14675,7 +14675,7 @@
         <v>2.0619999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>78</v>
       </c>
@@ -14863,7 +14863,7 @@
         <v>198.76</v>
       </c>
     </row>
-    <row r="30" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D30" s="2" t="s">
         <v>20</v>
       </c>
@@ -15048,7 +15048,7 @@
         <v>3.129</v>
       </c>
     </row>
-    <row r="31" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>76</v>
       </c>
@@ -15236,7 +15236,7 @@
         <v>57.07</v>
       </c>
     </row>
-    <row r="32" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>75</v>
       </c>
@@ -15424,7 +15424,7 @@
         <v>59.4</v>
       </c>
     </row>
-    <row r="33" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>73</v>
       </c>
@@ -15612,7 +15612,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="34" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>71</v>
       </c>
@@ -15800,7 +15800,7 @@
         <v>440.10700000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15"/>
       <c r="B35" s="2" t="s">
         <v>69</v>
@@ -15989,7 +15989,7 @@
         <v>172.202</v>
       </c>
     </row>
-    <row r="36" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -16051,7 +16051,7 @@
       <c r="BK36" s="12"/>
       <c r="BL36" s="12"/>
     </row>
-    <row r="37" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>67</v>
       </c>
@@ -16116,7 +16116,7 @@
       <c r="BK37" s="12"/>
       <c r="BL37" s="12"/>
     </row>
-    <row r="38" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>66</v>
       </c>
@@ -16304,7 +16304,7 @@
         <v>4.343</v>
       </c>
     </row>
-    <row r="39" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>65</v>
       </c>
@@ -16492,7 +16492,7 @@
         <v>169.917</v>
       </c>
     </row>
-    <row r="40" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D40" s="2" t="s">
         <v>20</v>
       </c>
@@ -16677,7 +16677,7 @@
         <v>0.28299999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="2" t="s">
         <v>64</v>
       </c>
@@ -16865,7 +16865,7 @@
         <v>60.713000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>63</v>
       </c>
@@ -17053,7 +17053,7 @@
         <v>162.536</v>
       </c>
     </row>
-    <row r="43" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D43" s="2" t="s">
         <v>20</v>
       </c>
@@ -17238,7 +17238,7 @@
         <v>0.248</v>
       </c>
     </row>
-    <row r="44" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="2" t="s">
         <v>62</v>
       </c>
@@ -17426,7 +17426,7 @@
         <v>158.464</v>
       </c>
     </row>
-    <row r="45" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D45" s="2" t="s">
         <v>20</v>
       </c>
@@ -17611,7 +17611,7 @@
         <v>0.30499999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="2" t="s">
         <v>61</v>
       </c>
@@ -17799,7 +17799,7 @@
         <v>133.11099999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D47" s="2" t="s">
         <v>20</v>
       </c>
@@ -17984,7 +17984,7 @@
         <v>1.7230000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>60</v>
       </c>
@@ -18172,7 +18172,7 @@
         <v>115.813</v>
       </c>
     </row>
-    <row r="49" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D49" s="2" t="s">
         <v>20</v>
       </c>
@@ -18357,7 +18357,7 @@
         <v>0.19900000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
@@ -18419,7 +18419,7 @@
       <c r="BK50" s="12"/>
       <c r="BL50" s="12"/>
     </row>
-    <row r="51" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>58</v>
       </c>
@@ -18484,7 +18484,7 @@
       <c r="BK51" s="12"/>
       <c r="BL51" s="12"/>
     </row>
-    <row r="52" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>57</v>
       </c>
@@ -18672,7 +18672,7 @@
         <v>279.86799999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D53" s="2" t="s">
         <v>20</v>
       </c>
@@ -18857,7 +18857,7 @@
         <v>0.53800000000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
         <v>56</v>
       </c>
@@ -19045,7 +19045,7 @@
         <v>135.44399999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E55" s="5"/>
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
@@ -19107,7 +19107,7 @@
       <c r="BK55" s="12"/>
       <c r="BL55" s="12"/>
     </row>
-    <row r="56" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>54</v>
       </c>
@@ -19172,7 +19172,7 @@
       <c r="BK56" s="12"/>
       <c r="BL56" s="12"/>
     </row>
-    <row r="57" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>53</v>
       </c>
@@ -19360,7 +19360,7 @@
         <v>3.419</v>
       </c>
     </row>
-    <row r="58" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>52</v>
       </c>
@@ -19548,7 +19548,7 @@
         <v>2.3650000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>51</v>
       </c>
@@ -19736,7 +19736,7 @@
         <v>2.5150000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
@@ -19798,7 +19798,7 @@
       <c r="BK60" s="12"/>
       <c r="BL60" s="12"/>
     </row>
-    <row r="61" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>49</v>
       </c>
@@ -19863,7 +19863,7 @@
       <c r="BK61" s="12"/>
       <c r="BL61" s="12"/>
     </row>
-    <row r="62" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>48</v>
       </c>
@@ -20051,7 +20051,7 @@
         <v>30495.4</v>
       </c>
     </row>
-    <row r="63" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D63" s="2" t="s">
         <v>37</v>
       </c>
@@ -20236,7 +20236,7 @@
         <v>90.501000000000005</v>
       </c>
     </row>
-    <row r="64" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
         <v>47</v>
       </c>
@@ -20424,7 +20424,7 @@
         <v>18106.099999999999</v>
       </c>
     </row>
-    <row r="65" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D65" s="2" t="s">
         <v>37</v>
       </c>
@@ -20609,7 +20609,7 @@
         <v>53.732999999999997</v>
       </c>
     </row>
-    <row r="66" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
         <v>46</v>
       </c>
@@ -20797,7 +20797,7 @@
         <v>14617</v>
       </c>
     </row>
-    <row r="67" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D67" s="2" t="s">
         <v>37</v>
       </c>
@@ -20982,7 +20982,7 @@
         <v>43.378999999999998</v>
       </c>
     </row>
-    <row r="68" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
         <v>45</v>
       </c>
@@ -21170,7 +21170,7 @@
         <v>8833.5</v>
       </c>
     </row>
-    <row r="69" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D69" s="2" t="s">
         <v>37</v>
       </c>
@@ -21355,7 +21355,7 @@
         <v>26.215</v>
       </c>
     </row>
-    <row r="70" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C70" s="2" t="s">
         <v>44</v>
       </c>
@@ -21543,7 +21543,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="71" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D71" s="2" t="s">
         <v>37</v>
       </c>
@@ -21728,7 +21728,7 @@
         <v>0.22500000000000001</v>
       </c>
     </row>
-    <row r="72" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C72" s="2" t="s">
         <v>43</v>
       </c>
@@ -21916,7 +21916,7 @@
         <v>2564.4</v>
       </c>
     </row>
-    <row r="73" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D73" s="2" t="s">
         <v>37</v>
       </c>
@@ -22101,7 +22101,7 @@
         <v>7.61</v>
       </c>
     </row>
-    <row r="74" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C74" s="2" t="s">
         <v>42</v>
       </c>
@@ -22289,7 +22289,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row r="75" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D75" s="2" t="s">
         <v>37</v>
       </c>
@@ -22474,7 +22474,7 @@
         <v>3.6669999999999998</v>
       </c>
     </row>
-    <row r="76" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C76" s="2" t="s">
         <v>41</v>
       </c>
@@ -22662,7 +22662,7 @@
         <v>2897.1</v>
       </c>
     </row>
-    <row r="77" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D77" s="2" t="s">
         <v>37</v>
       </c>
@@ -22847,7 +22847,7 @@
         <v>8.5969999999999995</v>
       </c>
     </row>
-    <row r="78" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C78" s="2" t="s">
         <v>40</v>
       </c>
@@ -23035,7 +23035,7 @@
         <v>2060.1999999999998</v>
       </c>
     </row>
-    <row r="79" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D79" s="2" t="s">
         <v>37</v>
       </c>
@@ -23220,7 +23220,7 @@
         <v>6.1139999999999999</v>
       </c>
     </row>
-    <row r="80" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="2" t="s">
         <v>39</v>
       </c>
@@ -23408,7 +23408,7 @@
         <v>3450.2</v>
       </c>
     </row>
-    <row r="81" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D81" s="2" t="s">
         <v>37</v>
       </c>
@@ -23593,7 +23593,7 @@
         <v>10.239000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="2" t="s">
         <v>38</v>
       </c>
@@ -23781,7 +23781,7 @@
         <v>2591.6999999999998</v>
       </c>
     </row>
-    <row r="83" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D83" s="2" t="s">
         <v>37</v>
       </c>
@@ -23966,7 +23966,7 @@
         <v>7.6909999999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
@@ -24028,7 +24028,7 @@
       <c r="BK84" s="12"/>
       <c r="BL84" s="12"/>
     </row>
-    <row r="85" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>36</v>
       </c>
@@ -24093,7 +24093,7 @@
       <c r="BK85" s="12"/>
       <c r="BL85" s="12"/>
     </row>
-    <row r="86" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="2" t="s">
         <v>32</v>
       </c>
@@ -24281,7 +24281,7 @@
         <v>23476.1</v>
       </c>
     </row>
-    <row r="87" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D87" s="2" t="s">
         <v>20</v>
       </c>
@@ -24466,7 +24466,7 @@
         <v>4.024</v>
       </c>
     </row>
-    <row r="88" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B88" s="2" t="s">
         <v>31</v>
       </c>
@@ -24654,7 +24654,7 @@
         <v>5649.8</v>
       </c>
     </row>
-    <row r="89" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D89" s="2" t="s">
         <v>20</v>
       </c>
@@ -24839,7 +24839,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="90" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C90" s="2" t="s">
         <v>30</v>
       </c>
@@ -25027,7 +25027,7 @@
         <v>4330.8</v>
       </c>
     </row>
-    <row r="91" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D91" s="2" t="s">
         <v>20</v>
       </c>
@@ -25212,7 +25212,7 @@
         <v>3.2269999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C92" s="14" t="s">
         <v>29</v>
       </c>
@@ -25400,7 +25400,7 @@
         <v>1265.2</v>
       </c>
     </row>
-    <row r="93" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D93" s="2" t="s">
         <v>20</v>
       </c>
@@ -25585,7 +25585,7 @@
         <v>1.4870000000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
         <v>28</v>
       </c>
@@ -25773,7 +25773,7 @@
         <v>53.8</v>
       </c>
     </row>
-    <row r="95" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="2" t="s">
         <v>27</v>
       </c>
@@ -25961,7 +25961,7 @@
         <v>5547</v>
       </c>
     </row>
-    <row r="96" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D96" s="2" t="s">
         <v>20</v>
       </c>
@@ -26146,7 +26146,7 @@
         <v>3.3359999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
         <v>26</v>
       </c>
@@ -26334,7 +26334,7 @@
         <v>1925.2</v>
       </c>
     </row>
-    <row r="98" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D98" s="2" t="s">
         <v>20</v>
       </c>
@@ -26519,7 +26519,7 @@
         <v>2.5230000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C99" s="2" t="s">
         <v>25</v>
       </c>
@@ -26707,7 +26707,7 @@
         <v>3621.8</v>
       </c>
     </row>
-    <row r="100" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D100" s="2" t="s">
         <v>20</v>
       </c>
@@ -26892,7 +26892,7 @@
         <v>3.7719999999999998</v>
       </c>
     </row>
-    <row r="101" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="2" t="s">
         <v>24</v>
       </c>
@@ -27080,7 +27080,7 @@
         <v>-977</v>
       </c>
     </row>
-    <row r="102" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C102" s="2" t="s">
         <v>23</v>
       </c>
@@ -27268,7 +27268,7 @@
         <v>3538.4</v>
       </c>
     </row>
-    <row r="103" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D103" s="2" t="s">
         <v>20</v>
       </c>
@@ -27453,7 +27453,7 @@
         <v>3.3519999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C104" s="2" t="s">
         <v>22</v>
       </c>
@@ -27641,7 +27641,7 @@
         <v>4515.3999999999996</v>
       </c>
     </row>
-    <row r="105" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D105" s="2" t="s">
         <v>20</v>
       </c>
@@ -27826,7 +27826,7 @@
         <v>3.4119999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="2" t="s">
         <v>35</v>
       </c>
@@ -28014,7 +28014,7 @@
         <v>-755.9</v>
       </c>
     </row>
-    <row r="107" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E107" s="5"/>
       <c r="F107" s="5"/>
       <c r="G107" s="5"/>
@@ -28076,7 +28076,7 @@
       <c r="BK107" s="12"/>
       <c r="BL107" s="12"/>
     </row>
-    <row r="108" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
         <v>33</v>
       </c>
@@ -28141,7 +28141,7 @@
       <c r="BK108" s="12"/>
       <c r="BL108" s="12"/>
     </row>
-    <row r="109" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="2" t="s">
         <v>32</v>
       </c>
@@ -28329,7 +28329,7 @@
         <v>16882.099999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D110" s="2" t="s">
         <v>20</v>
       </c>
@@ -28514,7 +28514,7 @@
         <v>1.9930000000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="2" t="s">
         <v>31</v>
       </c>
@@ -28702,7 +28702,7 @@
         <v>4378.8999999999996</v>
       </c>
     </row>
-    <row r="112" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D112" s="2" t="s">
         <v>20</v>
       </c>
@@ -28887,7 +28887,7 @@
         <v>1.5660000000000001</v>
       </c>
     </row>
-    <row r="113" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C113" s="2" t="s">
         <v>30</v>
       </c>
@@ -29075,7 +29075,7 @@
         <v>3723.6</v>
       </c>
     </row>
-    <row r="114" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D114" s="2" t="s">
         <v>20</v>
       </c>
@@ -29260,7 +29260,7 @@
         <v>2.3330000000000002</v>
       </c>
     </row>
-    <row r="115" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C115" s="2" t="s">
         <v>29</v>
       </c>
@@ -29448,7 +29448,7 @@
         <v>662.3</v>
       </c>
     </row>
-    <row r="116" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D116" s="2" t="s">
         <v>20</v>
       </c>
@@ -29633,7 +29633,7 @@
         <v>-1.149</v>
       </c>
     </row>
-    <row r="117" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C117" s="2" t="s">
         <v>28</v>
       </c>
@@ -29821,7 +29821,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="118" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="2" t="s">
         <v>27</v>
       </c>
@@ -30009,7 +30009,7 @@
         <v>3555.2</v>
       </c>
     </row>
-    <row r="119" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C119" s="2" t="s">
         <v>26</v>
       </c>
@@ -30197,7 +30197,7 @@
         <v>1363.5</v>
       </c>
     </row>
-    <row r="120" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C120" s="2" t="s">
         <v>25</v>
       </c>
@@ -30385,7 +30385,7 @@
         <v>2186.3000000000002</v>
       </c>
     </row>
-    <row r="121" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D121" s="2" t="s">
         <v>20</v>
       </c>
@@ -30570,7 +30570,7 @@
         <v>0.67200000000000004</v>
       </c>
     </row>
-    <row r="122" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B122" s="2" t="s">
         <v>24</v>
       </c>
@@ -30758,7 +30758,7 @@
         <v>-1336.4</v>
       </c>
     </row>
-    <row r="123" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C123" s="2" t="s">
         <v>23</v>
       </c>
@@ -30946,7 +30946,7 @@
         <v>3081.2</v>
       </c>
     </row>
-    <row r="124" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D124" s="2" t="s">
         <v>20</v>
       </c>
@@ -31131,7 +31131,7 @@
         <v>1.7370000000000001</v>
       </c>
     </row>
-    <row r="125" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C125" s="2" t="s">
         <v>22</v>
       </c>
@@ -31319,7 +31319,7 @@
         <v>4417.6000000000004</v>
       </c>
     </row>
-    <row r="126" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -31507,12 +31507,12 @@
         <v>2.2570000000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="130" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="73" t="s">
         <v>18</v>
       </c>
@@ -31520,10 +31520,10 @@
       <c r="C130" s="73"/>
       <c r="D130" s="73"/>
     </row>
-    <row r="131" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C131" s="6"/>
     </row>
-    <row r="132" spans="1:64" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:64" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>17</v>
       </c>
@@ -31541,7 +31541,7 @@
       <c r="P132" s="7"/>
       <c r="Q132" s="7"/>
     </row>
-    <row r="133" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C133" s="6"/>
       <c r="E133" s="5"/>
       <c r="G133" s="5"/>
@@ -31556,12 +31556,12 @@
       <c r="P133" s="5"/>
       <c r="Q133" s="5"/>
     </row>
-    <row r="134" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="3"/>
@@ -31641,21 +31641,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35EE37A-6DA7-464E-B4F9-9D022FBE10B3}">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B60" sqref="B60"/>
+      <selection pane="bottomRight" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="34" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="34" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -31708,7 +31708,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44286</v>
       </c>
@@ -31761,7 +31761,7 @@
         <v>6.2329999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44377</v>
       </c>
@@ -31814,7 +31814,7 @@
         <v>5.9329999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44469</v>
       </c>
@@ -31867,7 +31867,7 @@
         <v>5.0659999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44561</v>
       </c>
@@ -31920,7 +31920,7 @@
         <v>4.1660000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44651</v>
       </c>
@@ -31973,7 +31973,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44742</v>
       </c>
@@ -32026,7 +32026,7 @@
         <v>3.633</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44834</v>
       </c>
@@ -32080,7 +32080,7 @@
       </c>
       <c r="R8" s="33"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44926</v>
       </c>
@@ -32133,7 +32133,7 @@
         <v>3.5659999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45016</v>
       </c>
@@ -32186,7 +32186,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45107</v>
       </c>
@@ -32239,7 +32239,7 @@
         <v>3.5659999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45199</v>
       </c>
@@ -32292,7 +32292,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45291</v>
       </c>
@@ -32345,7 +32345,7 @@
         <v>3.7330000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45382</v>
       </c>
@@ -32398,7 +32398,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45473</v>
       </c>
@@ -32451,7 +32451,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45565</v>
       </c>
@@ -32504,7 +32504,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45657</v>
       </c>
@@ -32557,7 +32557,7 @@
         <v>4.1849999999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45747</v>
       </c>
@@ -32610,7 +32610,7 @@
         <v>4.2290000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45838</v>
       </c>
@@ -32663,7 +32663,7 @@
         <v>4.2590000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45930</v>
       </c>
@@ -32716,7 +32716,7 @@
         <v>4.2939999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>46022</v>
       </c>
@@ -32769,7 +32769,7 @@
         <v>4.3250000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>46112</v>
       </c>
@@ -32822,7 +32822,7 @@
         <v>4.3470000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>46203</v>
       </c>
@@ -32875,7 +32875,7 @@
         <v>4.3609999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>46295</v>
       </c>
@@ -32928,7 +32928,7 @@
         <v>4.37</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>46387</v>
       </c>
@@ -32981,7 +32981,7 @@
         <v>4.3769999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>46477</v>
       </c>
@@ -33034,7 +33034,7 @@
         <v>4.3819999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>46568</v>
       </c>
@@ -33087,7 +33087,7 @@
         <v>4.3890000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>46660</v>
       </c>
@@ -33140,7 +33140,7 @@
         <v>4.3979999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>46752</v>
       </c>
@@ -33193,7 +33193,7 @@
         <v>4.4029999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>46843</v>
       </c>
@@ -33246,7 +33246,7 @@
         <v>4.4059999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>46934</v>
       </c>
@@ -33299,7 +33299,7 @@
         <v>4.4059999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>47026</v>
       </c>
@@ -33352,7 +33352,7 @@
         <v>4.4039999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>47118</v>
       </c>
@@ -33405,7 +33405,7 @@
         <v>4.399</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>47208</v>
       </c>
@@ -33458,7 +33458,7 @@
         <v>4.3929999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>47299</v>
       </c>
@@ -33511,7 +33511,7 @@
         <v>4.3869999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>47391</v>
       </c>
@@ -33564,7 +33564,7 @@
         <v>4.3819999999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>47483</v>
       </c>
@@ -33617,7 +33617,7 @@
         <v>4.3789999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>47573</v>
       </c>
@@ -33670,7 +33670,7 @@
         <v>4.3780000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>47664</v>
       </c>
@@ -33723,7 +33723,7 @@
         <v>4.3769999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>47756</v>
       </c>
@@ -33776,7 +33776,7 @@
         <v>4.375</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>47848</v>
       </c>
@@ -33829,7 +33829,7 @@
         <v>4.3739999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>47938</v>
       </c>
@@ -33882,7 +33882,7 @@
         <v>4.3730000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>48029</v>
       </c>
@@ -33935,7 +33935,7 @@
         <v>4.3710000000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>48121</v>
       </c>
@@ -33988,7 +33988,7 @@
         <v>4.37</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>48213</v>
       </c>
@@ -34041,7 +34041,7 @@
         <v>4.3680000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>48304</v>
       </c>
@@ -34094,7 +34094,7 @@
         <v>4.367</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>48395</v>
       </c>
@@ -34147,7 +34147,7 @@
         <v>4.3639999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>48487</v>
       </c>
@@ -34200,7 +34200,7 @@
         <v>4.3609999999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48579</v>
       </c>
@@ -34253,7 +34253,7 @@
         <v>4.3570000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48669</v>
       </c>
@@ -34306,7 +34306,7 @@
         <v>4.3550000000000004</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>48760</v>
       </c>
@@ -34359,7 +34359,7 @@
         <v>4.351</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>48852</v>
       </c>
@@ -34412,7 +34412,7 @@
         <v>4.3470000000000004</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>48944</v>
       </c>
@@ -34465,7 +34465,7 @@
         <v>4.343</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>49034</v>
       </c>
@@ -34518,7 +34518,7 @@
         <v>4.34</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>49125</v>
       </c>
@@ -34571,7 +34571,7 @@
         <v>4.3360000000000003</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>49217</v>
       </c>
@@ -34622,271 +34622,6 @@
       </c>
       <c r="Q56" s="55">
         <v>4.3319999999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A57" s="1">
-        <v>49309</v>
-      </c>
-      <c r="B57" s="53">
-        <v>43326.8</v>
-      </c>
-      <c r="C57" s="53">
-        <v>28122.2</v>
-      </c>
-      <c r="D57" s="53">
-        <v>28263.5</v>
-      </c>
-      <c r="E57" s="53">
-        <v>43544.5</v>
-      </c>
-      <c r="F57" s="55">
-        <v>151.851</v>
-      </c>
-      <c r="G57" s="55">
-        <v>154.066</v>
-      </c>
-      <c r="H57" s="53">
-        <v>29899.7</v>
-      </c>
-      <c r="I57" s="53">
-        <v>19690.099999999999</v>
-      </c>
-      <c r="J57" s="53">
-        <v>4047.3</v>
-      </c>
-      <c r="K57" s="53">
-        <v>1517</v>
-      </c>
-      <c r="L57" s="53">
-        <v>2527.8000000000002</v>
-      </c>
-      <c r="M57" s="53">
-        <v>6732.6</v>
-      </c>
-      <c r="N57" s="53">
-        <v>2343.6</v>
-      </c>
-      <c r="O57" s="53">
-        <v>4389</v>
-      </c>
-      <c r="P57" s="55">
-        <v>395.78699999999998</v>
-      </c>
-      <c r="Q57" s="55">
-        <v>4.3289999999999997</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A58" s="1">
-        <v>49399</v>
-      </c>
-      <c r="B58" s="53">
-        <v>43731.199999999997</v>
-      </c>
-      <c r="C58" s="53">
-        <v>28245.1</v>
-      </c>
-      <c r="D58" s="53">
-        <v>28387</v>
-      </c>
-      <c r="E58" s="53">
-        <v>43950.9</v>
-      </c>
-      <c r="F58" s="55">
-        <v>152.589</v>
-      </c>
-      <c r="G58" s="55">
-        <v>154.827</v>
-      </c>
-      <c r="H58" s="53">
-        <v>30207</v>
-      </c>
-      <c r="I58" s="53">
-        <v>19796.2</v>
-      </c>
-      <c r="J58" s="53">
-        <v>4048.8</v>
-      </c>
-      <c r="K58" s="53">
-        <v>1517.9</v>
-      </c>
-      <c r="L58" s="53">
-        <v>2528.5</v>
-      </c>
-      <c r="M58" s="53">
-        <v>6779.2</v>
-      </c>
-      <c r="N58" s="53">
-        <v>2356.9</v>
-      </c>
-      <c r="O58" s="53">
-        <v>4422.3999999999996</v>
-      </c>
-      <c r="P58" s="55">
-        <v>397.995</v>
-      </c>
-      <c r="Q58" s="55">
-        <v>4.3250000000000002</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A59" s="1">
-        <v>49490</v>
-      </c>
-      <c r="B59" s="53">
-        <v>44138.8</v>
-      </c>
-      <c r="C59" s="53">
-        <v>28368.1</v>
-      </c>
-      <c r="D59" s="53">
-        <v>28510.7</v>
-      </c>
-      <c r="E59" s="53">
-        <v>44360.6</v>
-      </c>
-      <c r="F59" s="55">
-        <v>153.33000000000001</v>
-      </c>
-      <c r="G59" s="55">
-        <v>155.59200000000001</v>
-      </c>
-      <c r="H59" s="53">
-        <v>30516</v>
-      </c>
-      <c r="I59" s="53">
-        <v>19902.099999999999</v>
-      </c>
-      <c r="J59" s="53">
-        <v>4050.3</v>
-      </c>
-      <c r="K59" s="53">
-        <v>1518.8</v>
-      </c>
-      <c r="L59" s="53">
-        <v>2529.1</v>
-      </c>
-      <c r="M59" s="53">
-        <v>6826.2</v>
-      </c>
-      <c r="N59" s="53">
-        <v>2370.1999999999998</v>
-      </c>
-      <c r="O59" s="53">
-        <v>4456</v>
-      </c>
-      <c r="P59" s="55">
-        <v>400.21600000000001</v>
-      </c>
-      <c r="Q59" s="55">
-        <v>4.3209999999999997</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A60" s="1">
-        <v>49582</v>
-      </c>
-      <c r="B60" s="53">
-        <v>44549.3</v>
-      </c>
-      <c r="C60" s="53">
-        <v>28491.1</v>
-      </c>
-      <c r="D60" s="53">
-        <v>28634.3</v>
-      </c>
-      <c r="E60" s="53">
-        <v>44773.1</v>
-      </c>
-      <c r="F60" s="55">
-        <v>154.07499999999999</v>
-      </c>
-      <c r="G60" s="55">
-        <v>156.36099999999999</v>
-      </c>
-      <c r="H60" s="53">
-        <v>30827</v>
-      </c>
-      <c r="I60" s="53">
-        <v>20007.8</v>
-      </c>
-      <c r="J60" s="53">
-        <v>4051.7</v>
-      </c>
-      <c r="K60" s="53">
-        <v>1519.7</v>
-      </c>
-      <c r="L60" s="53">
-        <v>2529.6999999999998</v>
-      </c>
-      <c r="M60" s="53">
-        <v>6873.5</v>
-      </c>
-      <c r="N60" s="53">
-        <v>2383.6999999999998</v>
-      </c>
-      <c r="O60" s="53">
-        <v>4489.8</v>
-      </c>
-      <c r="P60" s="55">
-        <v>402.45</v>
-      </c>
-      <c r="Q60" s="55">
-        <v>4.3170000000000002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A61" s="1">
-        <v>49674</v>
-      </c>
-      <c r="B61" s="53">
-        <v>44962.6</v>
-      </c>
-      <c r="C61" s="53">
-        <v>28614</v>
-      </c>
-      <c r="D61" s="53">
-        <v>28757.7</v>
-      </c>
-      <c r="E61" s="53">
-        <v>45188.5</v>
-      </c>
-      <c r="F61" s="55">
-        <v>154.82300000000001</v>
-      </c>
-      <c r="G61" s="55">
-        <v>157.13499999999999</v>
-      </c>
-      <c r="H61" s="53">
-        <v>31138.6</v>
-      </c>
-      <c r="I61" s="53">
-        <v>20112.400000000001</v>
-      </c>
-      <c r="J61" s="53">
-        <v>4053.4</v>
-      </c>
-      <c r="K61" s="53">
-        <v>1520.8</v>
-      </c>
-      <c r="L61" s="53">
-        <v>2530.1999999999998</v>
-      </c>
-      <c r="M61" s="53">
-        <v>6921.6</v>
-      </c>
-      <c r="N61" s="53">
-        <v>2397.6</v>
-      </c>
-      <c r="O61" s="53">
-        <v>4524</v>
-      </c>
-      <c r="P61" s="55">
-        <v>404.697</v>
-      </c>
-      <c r="Q61" s="55">
-        <v>4.3140000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -34900,12 +34635,12 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="A14" sqref="A14:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>158</v>
       </c>
@@ -34937,7 +34672,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2023</v>
       </c>
@@ -34969,7 +34704,7 @@
         <v>36.145000000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -35001,7 +34736,7 @@
         <v>35.369999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2025</v>
       </c>
@@ -35033,7 +34768,7 @@
         <v>33.424999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -35065,7 +34800,7 @@
         <v>32.450000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2027</v>
       </c>
@@ -35097,7 +34832,7 @@
         <v>33.164999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2028</v>
       </c>
@@ -35129,7 +34864,7 @@
         <v>35.090000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2029</v>
       </c>
@@ -35161,7 +34896,7 @@
         <v>37.164999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -35193,7 +34928,7 @@
         <v>39.784999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2031</v>
       </c>
@@ -35225,7 +34960,7 @@
         <v>44.73</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -35254,7 +34989,7 @@
         <v>54.478999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2033</v>
       </c>
@@ -35283,7 +35018,7 @@
         <v>56.115000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2034</v>
       </c>
@@ -35312,36 +35047,7 @@
         <v>57.764000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>2035</v>
-      </c>
-      <c r="B14" s="59">
-        <v>5391.2759999999998</v>
-      </c>
-      <c r="C14" s="61">
-        <v>4412.8320000000003</v>
-      </c>
-      <c r="D14" s="61">
-        <v>496.29000000000008</v>
-      </c>
-      <c r="E14" s="61">
-        <v>517.11500000000001</v>
-      </c>
-      <c r="F14" s="61">
-        <v>2605.1819999999998</v>
-      </c>
-      <c r="G14" s="58">
-        <v>2166.35</v>
-      </c>
-      <c r="H14" s="58">
-        <v>1025.287</v>
-      </c>
-      <c r="I14" s="58">
-        <v>59.441000000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="57"/>
       <c r="D18" s="57"/>
       <c r="E18" s="57"/>
@@ -35355,7 +35061,7 @@
       <c r="M18" s="57"/>
       <c r="N18" s="57"/>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19" s="57"/>
       <c r="D19" s="57"/>
       <c r="E19" s="57"/>
@@ -35369,7 +35075,7 @@
       <c r="M19" s="57"/>
       <c r="N19" s="57"/>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20" s="57"/>
       <c r="D20" s="57"/>
       <c r="E20" s="57"/>
@@ -35383,7 +35089,7 @@
       <c r="M20" s="57"/>
       <c r="N20" s="57"/>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C21" s="57"/>
       <c r="D21" s="57"/>
       <c r="E21" s="57"/>
@@ -35397,7 +35103,7 @@
       <c r="M21" s="57"/>
       <c r="N21" s="57"/>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
@@ -35421,13 +35127,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86381FD6-3DA6-864B-ACAE-10D968FEABB3}">
   <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -35438,7 +35144,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43921</v>
       </c>
@@ -35449,7 +35155,7 @@
         <v>3.8639999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44012</v>
       </c>
@@ -35460,7 +35166,7 @@
         <v>3.2149999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44104</v>
       </c>
@@ -35471,7 +35177,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44196</v>
       </c>
@@ -35482,7 +35188,7 @@
         <v>3.7440000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44286</v>
       </c>
@@ -35493,7 +35199,7 @@
         <v>3.734</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44377</v>
       </c>
@@ -35504,7 +35210,7 @@
         <v>3.7170000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44469</v>
       </c>
@@ -35515,7 +35221,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44561</v>
       </c>
@@ -35526,7 +35232,7 @@
         <v>3.7509999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44651</v>
       </c>
@@ -35537,7 +35243,7 @@
         <v>9.2159999999999993</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44742</v>
       </c>
@@ -35548,7 +35254,7 @@
         <v>9.843</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44834</v>
       </c>
@@ -35559,7 +35265,7 @@
         <v>7.6760000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44926</v>
       </c>
@@ -35570,7 +35276,7 @@
         <v>5.7149999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45016</v>
       </c>
@@ -35581,7 +35287,7 @@
         <v>4.9859999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45107</v>
       </c>
@@ -35592,7 +35298,7 @@
         <v>4.2220000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45199</v>
       </c>
@@ -35603,7 +35309,7 @@
         <v>3.7879999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45291</v>
       </c>
@@ -35614,7 +35320,7 @@
         <v>3.6309999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45382</v>
       </c>
@@ -35625,7 +35331,7 @@
         <v>3.5049999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45473</v>
       </c>
@@ -35636,7 +35342,7 @@
         <v>3.4809999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45565</v>
       </c>
@@ -35647,7 +35353,7 @@
         <v>3.5430000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45657</v>
       </c>
@@ -35658,7 +35364,7 @@
         <v>3.633</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45747</v>
       </c>
@@ -35669,7 +35375,7 @@
         <v>3.8759999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45838</v>
       </c>
@@ -35680,7 +35386,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45930</v>
       </c>
@@ -35691,7 +35397,7 @@
         <v>4.0709999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>46022</v>
       </c>
@@ -35702,7 +35408,7 @@
         <v>4.0750000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>46112</v>
       </c>
@@ -35713,7 +35419,7 @@
         <v>4.032</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>46203</v>
       </c>
@@ -35724,7 +35430,7 @@
         <v>3.9910000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>46295</v>
       </c>
@@ -35735,7 +35441,7 @@
         <v>3.9529999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>46387</v>
       </c>
@@ -35746,7 +35452,7 @@
         <v>3.923</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>46477</v>
       </c>
@@ -35757,7 +35463,7 @@
         <v>3.8959999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>46568</v>
       </c>
@@ -35768,7 +35474,7 @@
         <v>3.891</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>46660</v>
       </c>
@@ -35779,7 +35485,7 @@
         <v>3.8620000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>46752</v>
       </c>
@@ -35790,7 +35496,7 @@
         <v>3.8380000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>46843</v>
       </c>
@@ -35801,7 +35507,7 @@
         <v>3.8039999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>46934</v>
       </c>
@@ -35812,7 +35518,7 @@
         <v>3.7970000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>47026</v>
       </c>
@@ -35823,7 +35529,7 @@
         <v>3.78</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>47118</v>
       </c>
@@ -35834,7 +35540,7 @@
         <v>3.766</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>47208</v>
       </c>
@@ -35845,7 +35551,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>47299</v>
       </c>
@@ -35856,7 +35562,7 @@
         <v>3.746</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>47391</v>
       </c>
@@ -35867,7 +35573,7 @@
         <v>3.7570000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>47483</v>
       </c>
@@ -35878,7 +35584,7 @@
         <v>3.7709999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>47573</v>
       </c>
@@ -35889,7 +35595,7 @@
         <v>3.7749999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>47664</v>
       </c>
@@ -35900,7 +35606,7 @@
         <v>3.7810000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>47756</v>
       </c>
@@ -35911,7 +35617,7 @@
         <v>3.7879999999999998</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>47848</v>
       </c>
@@ -35922,7 +35628,7 @@
         <v>3.7879999999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>47938</v>
       </c>
@@ -35933,7 +35639,7 @@
         <v>3.8069999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>48029</v>
       </c>
@@ -35944,7 +35650,7 @@
         <v>3.7909999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>48121</v>
       </c>
@@ -35955,7 +35661,7 @@
         <v>3.7909999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48213</v>
       </c>
@@ -35966,7 +35672,7 @@
         <v>3.7839999999999998</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" s="29">
         <v>2.3690000000000002</v>
       </c>
@@ -35974,7 +35680,7 @@
         <v>3.79</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="29">
         <v>2.37</v>
       </c>
@@ -35982,7 +35688,7 @@
         <v>3.7909999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" s="29">
         <v>2.371</v>
       </c>
@@ -35990,7 +35696,7 @@
         <v>3.7869999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="29">
         <v>2.4249999999999998</v>
       </c>
@@ -36011,23 +35717,23 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.375" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="50.33203125" customWidth="1"/>
+    <col min="3" max="3" width="50.375" customWidth="1"/>
     <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="19.58203125" customWidth="1"/>
+    <col min="5" max="5" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
         <v>216</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>273</v>
       </c>
@@ -36041,7 +35747,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -36059,7 +35765,7 @@
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>271</v>
       </c>
@@ -36077,7 +35783,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>272</v>
       </c>
@@ -36095,7 +35801,7 @@
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>241</v>
       </c>
@@ -36113,7 +35819,7 @@
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>243</v>
       </c>
@@ -36133,7 +35839,7 @@
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>247</v>
       </c>
@@ -36153,7 +35859,7 @@
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>250</v>
       </c>
@@ -36171,7 +35877,7 @@
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>252</v>
       </c>
@@ -36193,7 +35899,7 @@
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>257</v>
       </c>
@@ -36211,7 +35917,7 @@
       <c r="G11" s="30"/>
       <c r="H11" s="30"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>260</v>
       </c>
@@ -36229,7 +35935,7 @@
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>262</v>
       </c>
@@ -36247,7 +35953,7 @@
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>264</v>
       </c>
@@ -36265,7 +35971,7 @@
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>266</v>
       </c>
@@ -36283,7 +35989,7 @@
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>268</v>
       </c>
@@ -36301,7 +36007,7 @@
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>269</v>
       </c>
@@ -36319,7 +36025,7 @@
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>270</v>
       </c>
@@ -36337,14 +36043,14 @@
       <c r="G18" s="30"/>
       <c r="H18" s="30"/>
     </row>
-    <row r="21" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
         <v>226</v>
       </c>
       <c r="B21" s="69"/>
       <c r="C21" s="69"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>217</v>
       </c>
@@ -36352,7 +36058,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>219</v>
       </c>
@@ -36360,7 +36066,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>221</v>
       </c>
@@ -36368,7 +36074,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>223</v>
       </c>
@@ -36376,14 +36082,14 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="69" t="s">
         <v>225</v>
       </c>
       <c r="B26" s="69"/>
       <c r="C26" s="69"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>227</v>
       </c>
@@ -36391,7 +36097,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>228</v>
       </c>
@@ -36399,7 +36105,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>229</v>
       </c>
@@ -36407,7 +36113,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>230</v>
       </c>
@@ -36434,9 +36140,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36444,7 +36150,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>197</v>
       </c>
@@ -36452,7 +36158,7 @@
         <v>0.66513142470107067</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>198</v>
       </c>
@@ -36460,7 +36166,7 @@
         <v>0.66892566614130466</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>199</v>
       </c>
@@ -36468,7 +36174,7 @@
         <v>0.65283836530948725</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>200</v>
       </c>
@@ -36476,7 +36182,7 @@
         <v>0.65953557146217701</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>201</v>
       </c>
@@ -36484,7 +36190,7 @@
         <v>0.66058231423538405</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>202</v>
       </c>
@@ -36492,7 +36198,7 @@
         <v>0.6749214177505789</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>203</v>
       </c>
@@ -36500,7 +36206,7 @@
         <v>0.68242012696430432</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>204</v>
       </c>
@@ -36508,7 +36214,7 @@
         <v>0.6730637268687778</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>205</v>
       </c>
@@ -36516,7 +36222,7 @@
         <v>0.66424643423393748</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>206</v>
       </c>
@@ -36524,7 +36230,7 @@
         <v>0.67846773573296415</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>207</v>
       </c>
@@ -36532,7 +36238,7 @@
         <v>0.76648081779484256</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>208</v>
       </c>
@@ -36540,7 +36246,7 @@
         <v>0.71094027669909299</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>209</v>
       </c>
@@ -36548,7 +36254,7 @@
         <v>0.75054511245142341</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>185</v>
       </c>
@@ -36556,7 +36262,7 @@
         <v>0.7533823239283487</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>186</v>
       </c>
@@ -36567,7 +36273,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>187</v>
       </c>
@@ -36575,7 +36281,7 @@
         <v>0.75196371818988605</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>188</v>
       </c>
@@ -36583,7 +36289,7 @@
         <v>0.75196371818988605</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>189</v>
       </c>
@@ -36591,7 +36297,7 @@
         <v>0.75196371818988605</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>190</v>
       </c>
@@ -36599,7 +36305,7 @@
         <v>0.75196371818988605</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>191</v>
       </c>
@@ -36607,7 +36313,7 @@
         <v>0.67274689645476105</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>192</v>
       </c>
@@ -36615,7 +36321,7 @@
         <v>0.67274689645476138</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>193</v>
       </c>
@@ -36623,7 +36329,7 @@
         <v>0.67274689645476138</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>194</v>
       </c>
@@ -36631,7 +36337,7 @@
         <v>0.67274689645476138</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>195</v>
       </c>
@@ -36639,7 +36345,7 @@
         <v>0.67274689645476138</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -36647,7 +36353,7 @@
         <v>0.67274689645476138</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>210</v>
       </c>
@@ -36668,9 +36374,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>158</v>
       </c>
@@ -36678,7 +36384,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="27">
         <v>2019</v>
       </c>
@@ -36686,7 +36392,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="27">
         <v>2020</v>
       </c>
@@ -36694,7 +36400,7 @@
         <v>0.70499999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="27">
         <v>2021</v>
       </c>
@@ -36702,7 +36408,7 @@
         <v>0.752</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="27">
         <v>2022</v>
       </c>
@@ -36710,7 +36416,7 @@
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="27">
         <v>2023</v>
       </c>
@@ -36718,7 +36424,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="27">
         <v>2024</v>
       </c>
@@ -36726,7 +36432,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="27">
         <v>2025</v>
       </c>
@@ -36734,7 +36440,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="27">
         <v>2026</v>
       </c>
@@ -36742,7 +36448,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>2027</v>
       </c>
@@ -36750,7 +36456,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="27">
         <v>2028</v>
       </c>
@@ -36758,7 +36464,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>2029</v>
       </c>
@@ -36778,7 +36484,7 @@
       <c r="O12" s="27"/>
       <c r="P12" s="27"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="27">
         <v>2030</v>
       </c>
@@ -36811,9 +36517,9 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -36830,7 +36536,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -36852,7 +36558,7 @@
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -36873,7 +36579,7 @@
       <c r="K3" s="26"/>
       <c r="L3" s="26"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -36890,7 +36596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>188</v>
       </c>
@@ -36907,7 +36613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -36924,7 +36630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>190</v>
       </c>
@@ -36941,7 +36647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>191</v>
       </c>
@@ -36958,7 +36664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>192</v>
       </c>
@@ -36975,7 +36681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>193</v>
       </c>
@@ -36992,7 +36698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>194</v>
       </c>
@@ -37009,7 +36715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>195</v>
       </c>
@@ -37026,7 +36732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>196</v>
       </c>
@@ -37056,9 +36762,9 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -37105,7 +36811,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2021</v>
       </c>
@@ -37154,7 +36860,7 @@
         <v>181.506</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -37182,7 +36888,7 @@
         <v>1.7549999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2023</v>
       </c>
@@ -37210,7 +36916,7 @@
         <v>0.67600000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2024</v>
       </c>
@@ -37255,7 +36961,7 @@
         <v>0.53100000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -37300,7 +37006,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2026</v>
       </c>
@@ -37345,7 +37051,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2027</v>
       </c>
@@ -37390,7 +37096,7 @@
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2028</v>
       </c>
@@ -37435,7 +37141,7 @@
         <v>0.52700000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2029</v>
       </c>
@@ -37480,7 +37186,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2030</v>
       </c>
@@ -37525,7 +37231,7 @@
         <v>0.53500000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2031</v>
       </c>

</xml_diff>